<commit_message>
additional test cases, handled case of all zeroes
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subogupt.ORADEV\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyGitProject\TokBoxBookStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Book price</t>
   </si>
@@ -46,13 +46,30 @@
   <si>
     <t>Remaining amount</t>
   </si>
+  <si>
+    <t>Check for the high lighted rows</t>
+  </si>
+  <si>
+    <t>Last highlight rows contains the remaining amount and purchased book count</t>
+  </si>
+  <si>
+    <t>Enter values above</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,15 +118,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -385,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,378 +437,898 @@
     <col min="9" max="11" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>H2</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1">
         <f>K2-A2</f>
-        <v>95</v>
+        <v>225</v>
       </c>
       <c r="H2" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="J2" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>IF(A2-$I$2&lt;$J$2,$J$2,A2-$I$2)</f>
-        <v>10</v>
+        <f t="shared" ref="A3:A40" si="0">IF(A2-$I$2&lt;$J$2,$J$2,A2-$I$2)</f>
+        <v>21.5</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1">
         <f>C2-A3</f>
-        <v>85</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>203.5</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f>IF(A3-$I$2&lt;$J$2,$J$2,A3-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C26" si="0">C3-A4</f>
-        <v>75</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C4:C40" si="1">C3-A4</f>
+        <v>183.5</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>IF(A4-$I$2&lt;$J$2,$J$2,A4-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>163.5</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f>IF(A5-$I$2&lt;$J$2,$J$2,A5-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>143.5</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>IF(A6-$I$2&lt;$J$2,$J$2,A6-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>123.5</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f>IF(A7-$I$2&lt;$J$2,$J$2,A7-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <f>IF(A8-$I$2&lt;$J$2,$J$2,A8-$I$2)</f>
-        <v>10</v>
-      </c>
-      <c r="B9" s="2">
+        <f t="shared" si="1"/>
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B9" s="3">
         <v>8</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>83.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f>IF(A9-$I$2&lt;$J$2,$J$2,A9-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>63.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f>IF(A10-$I$2&lt;$J$2,$J$2,A10-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f>IF(A11-$I$2&lt;$J$2,$J$2,A11-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="0"/>
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f>IF(A12-$I$2&lt;$J$2,$J$2,A12-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="0"/>
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f>IF(A13-$I$2&lt;$J$2,$J$2,A13-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="0"/>
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-16.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f>IF(A14-$I$2&lt;$J$2,$J$2,A14-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="0"/>
-        <v>-35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-36.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f>IF(A15-$I$2&lt;$J$2,$J$2,A15-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>15</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="0"/>
-        <v>-45</v>
+        <f t="shared" si="1"/>
+        <v>-56.5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f>IF(A16-$I$2&lt;$J$2,$J$2,A16-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
         <v>16</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="0"/>
-        <v>-55</v>
+        <f t="shared" si="1"/>
+        <v>-76.5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f>IF(A17-$I$2&lt;$J$2,$J$2,A17-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B18" s="1">
         <v>17</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="0"/>
-        <v>-65</v>
+        <f t="shared" si="1"/>
+        <v>-96.5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f>IF(A18-$I$2&lt;$J$2,$J$2,A18-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>18</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="0"/>
-        <v>-75</v>
+        <f t="shared" si="1"/>
+        <v>-116.5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f>IF(A19-$I$2&lt;$J$2,$J$2,A19-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
         <v>19</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="0"/>
-        <v>-85</v>
+        <f t="shared" si="1"/>
+        <v>-136.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f>IF(A20-$I$2&lt;$J$2,$J$2,A20-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="0"/>
-        <v>-95</v>
+        <f t="shared" si="1"/>
+        <v>-156.5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f>IF(A21-$I$2&lt;$J$2,$J$2,A21-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>21</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="0"/>
-        <v>-105</v>
+        <f t="shared" si="1"/>
+        <v>-176.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f>IF(A22-$I$2&lt;$J$2,$J$2,A22-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B23" s="1">
         <v>22</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="0"/>
-        <v>-115</v>
+        <f t="shared" si="1"/>
+        <v>-196.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f>IF(A23-$I$2&lt;$J$2,$J$2,A23-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B24" s="1">
         <v>23</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="0"/>
-        <v>-125</v>
+        <f t="shared" si="1"/>
+        <v>-216.5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f>IF(A24-$I$2&lt;$J$2,$J$2,A24-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B25" s="1">
         <v>24</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="0"/>
-        <v>-135</v>
+        <f t="shared" si="1"/>
+        <v>-236.5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f>IF(A25-$I$2&lt;$J$2,$J$2,A25-$I$2)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B26" s="1">
         <v>25</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="0"/>
-        <v>-145</v>
+        <f t="shared" si="1"/>
+        <v>-256.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B27" s="1">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="1"/>
+        <v>-276.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B28" s="1">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="1"/>
+        <v>-296.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B29" s="1">
+        <v>25</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="1"/>
+        <v>-316.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B30" s="1">
+        <v>25</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="1"/>
+        <v>-336.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B31" s="1">
+        <v>25</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="1"/>
+        <v>-356.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B32" s="1">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="1"/>
+        <v>-376.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B33" s="1">
+        <v>25</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="1"/>
+        <v>-396.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B34" s="1">
+        <v>25</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" si="1"/>
+        <v>-416.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B35" s="1">
+        <v>25</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" si="1"/>
+        <v>-436.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B36" s="1">
+        <v>25</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" si="1"/>
+        <v>-456.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B37" s="1">
+        <v>25</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="1"/>
+        <v>-476.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B38" s="1">
+        <v>25</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="1"/>
+        <v>-496.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B39" s="1">
+        <v>25</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="1"/>
+        <v>-516.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B40" s="1">
+        <v>25</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="1"/>
+        <v>-536.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <f t="shared" ref="A41:A64" si="2">IF(A40-$I$2&lt;$J$2,$J$2,A40-$I$2)</f>
+        <v>20</v>
+      </c>
+      <c r="B41" s="1">
+        <v>25</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" ref="C41:C64" si="3">C40-A41</f>
+        <v>-556.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B42" s="1">
+        <v>25</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="3"/>
+        <v>-576.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B43" s="1">
+        <v>25</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="3"/>
+        <v>-596.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B44" s="1">
+        <v>25</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="3"/>
+        <v>-616.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B45" s="1">
+        <v>25</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="3"/>
+        <v>-636.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B46" s="1">
+        <v>25</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="3"/>
+        <v>-656.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B47" s="1">
+        <v>25</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" si="3"/>
+        <v>-676.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B48" s="1">
+        <v>25</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="3"/>
+        <v>-696.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B49" s="1">
+        <v>25</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" si="3"/>
+        <v>-716.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B50" s="1">
+        <v>25</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" si="3"/>
+        <v>-736.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B51" s="1">
+        <v>25</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" si="3"/>
+        <v>-756.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B52" s="1">
+        <v>25</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" si="3"/>
+        <v>-776.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B53" s="1">
+        <v>25</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="3"/>
+        <v>-796.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B54" s="1">
+        <v>25</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="3"/>
+        <v>-816.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B55" s="1">
+        <v>25</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="3"/>
+        <v>-836.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B56" s="1">
+        <v>25</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" si="3"/>
+        <v>-856.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B57" s="1">
+        <v>25</v>
+      </c>
+      <c r="C57" s="1">
+        <f t="shared" si="3"/>
+        <v>-876.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B58" s="1">
+        <v>25</v>
+      </c>
+      <c r="C58" s="1">
+        <f t="shared" si="3"/>
+        <v>-896.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B59" s="1">
+        <v>25</v>
+      </c>
+      <c r="C59" s="1">
+        <f t="shared" si="3"/>
+        <v>-916.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B60" s="1">
+        <v>25</v>
+      </c>
+      <c r="C60" s="1">
+        <f t="shared" si="3"/>
+        <v>-936.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B61" s="1">
+        <v>25</v>
+      </c>
+      <c r="C61" s="1">
+        <f t="shared" si="3"/>
+        <v>-956.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B62" s="1">
+        <v>25</v>
+      </c>
+      <c r="C62" s="1">
+        <f t="shared" si="3"/>
+        <v>-976.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B63" s="1">
+        <v>25</v>
+      </c>
+      <c r="C63" s="1">
+        <f t="shared" si="3"/>
+        <v>-996.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B64" s="1">
+        <v>25</v>
+      </c>
+      <c r="C64" s="1">
+        <f t="shared" si="3"/>
+        <v>-1016.5</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C40 C65:C1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41:C64">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>